<commit_message>
Defined most(?) of the opcodes for XMOS->STM32.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS-&gt;STM32" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>Command</t>
   </si>
@@ -97,6 +97,84 @@
   </si>
   <si>
     <t>CMD/REPLY</t>
+  </si>
+  <si>
+    <t>OPCODE_6</t>
+  </si>
+  <si>
+    <t>OPCODE_5</t>
+  </si>
+  <si>
+    <t>OPCODE_4</t>
+  </si>
+  <si>
+    <t>OPCODE_3</t>
+  </si>
+  <si>
+    <t>OPCODE_2</t>
+  </si>
+  <si>
+    <t>OPCODE_1</t>
+  </si>
+  <si>
+    <t>OPCODE_0</t>
+  </si>
+  <si>
+    <t>Send over USB</t>
+  </si>
+  <si>
+    <t>Set ADC to 12-bit</t>
+  </si>
+  <si>
+    <t>Set ADC to 10-bit</t>
+  </si>
+  <si>
+    <t>Set ADC to 8-bit</t>
+  </si>
+  <si>
+    <t>Set ADC to 6-bit</t>
+  </si>
+  <si>
+    <t>Get RTC time</t>
+  </si>
+  <si>
+    <t>Get RTC date</t>
+  </si>
+  <si>
+    <t>Get ADC resolution</t>
+  </si>
+  <si>
+    <t>ADC resolution</t>
+  </si>
+  <si>
+    <t>2-bit</t>
+  </si>
+  <si>
+    <t>24-bit</t>
+  </si>
+  <si>
+    <t>Data width</t>
+  </si>
+  <si>
+    <t>Get DAC resolution</t>
+  </si>
+  <si>
+    <t>Set DAC to 12-bit</t>
+  </si>
+  <si>
+    <t>Set DAC to 8-bit</t>
+  </si>
+  <si>
+    <t>Output on DAC 0</t>
+  </si>
+  <si>
+    <t>Output on DAC 1</t>
+  </si>
+  <si>
+    <t>DAC resolution</t>
+  </si>
+  <si>
+    <t>1-bit</t>
   </si>
 </sst>
 </file>
@@ -435,329 +513,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
       <c r="B26">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
       <c r="B27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
       <c r="B28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
       <c r="B29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
       <c r="B30">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
       <c r="B31">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
       <c r="B32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
       <c r="B33">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
       <c r="B34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
       <c r="B35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
       <c r="B36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
       <c r="B37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
       <c r="B38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>46</v>
       </c>
@@ -868,13 +1101,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -907,6 +1147,27 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed the set ADC/DAC resolution commands to be one opcode each.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Command</t>
   </si>
@@ -123,18 +123,6 @@
     <t>Send over USB</t>
   </si>
   <si>
-    <t>Set ADC to 12-bit</t>
-  </si>
-  <si>
-    <t>Set ADC to 10-bit</t>
-  </si>
-  <si>
-    <t>Set ADC to 8-bit</t>
-  </si>
-  <si>
-    <t>Set ADC to 6-bit</t>
-  </si>
-  <si>
     <t>Get RTC time</t>
   </si>
   <si>
@@ -175,6 +163,18 @@
   </si>
   <si>
     <t>1-bit</t>
+  </si>
+  <si>
+    <t>Set ADC resolution</t>
+  </si>
+  <si>
+    <t>Set RTC time</t>
+  </si>
+  <si>
+    <t>Set RTC date</t>
+  </si>
+  <si>
+    <t>8-bit   ?</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,7 +623,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,150 +799,139 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Swapped get/set positions for RTC for consistency.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Command</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Get DAC resolution</t>
   </si>
   <si>
-    <t>Set DAC to 12-bit</t>
-  </si>
-  <si>
-    <t>Set DAC to 8-bit</t>
-  </si>
-  <si>
     <t>Output on DAC 0</t>
   </si>
   <si>
@@ -175,6 +169,9 @@
   </si>
   <si>
     <t>8-bit   ?</t>
+  </si>
+  <si>
+    <t>Set DAC resolution</t>
   </si>
 </sst>
 </file>
@@ -516,7 +513,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +812,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -832,15 +829,15 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>40</v>
@@ -848,10 +845,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -859,10 +856,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
@@ -870,10 +867,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
@@ -884,54 +881,53 @@
         <v>42</v>
       </c>
       <c r="B33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
         <v>45</v>
       </c>
-      <c r="B36">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>35</v>
       </c>
-      <c r="D36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added two UART opcodes to control the Arduino IO pins.
The data format is described in the manual.
The manual entry has all of the information, but isn't fully written up yet.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Command</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Set DAC resolution</t>
+  </si>
+  <si>
+    <t>Get IO pin status</t>
+  </si>
+  <si>
+    <t>Set IO pin state</t>
+  </si>
+  <si>
+    <t>5-bit cmd, 17-bit reply</t>
+  </si>
+  <si>
+    <t>17-bit</t>
   </si>
 </sst>
 </file>
@@ -513,7 +525,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,13 +933,25 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
       <c r="B37">
         <v>35</v>
       </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
       <c r="B38">
         <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 4 new opcodes to control U15 from the XMOS.
The data_widths arrays in the STM32 library also had not been updated with the additon of opcodes 35 and 36. That has been resolved.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Command</t>
   </si>
@@ -184,6 +184,30 @@
   </si>
   <si>
     <t>17-bit</t>
+  </si>
+  <si>
+    <t>Get U15 output pin X</t>
+  </si>
+  <si>
+    <t>Set U15 output pin X</t>
+  </si>
+  <si>
+    <t>Get U15 outputs</t>
+  </si>
+  <si>
+    <t>Set U15 outputs</t>
+  </si>
+  <si>
+    <t>3-bit cmd, 1-bit reply</t>
+  </si>
+  <si>
+    <t>4-bit cmd</t>
+  </si>
+  <si>
+    <t>8-bit reply</t>
+  </si>
+  <si>
+    <t>8-bit command</t>
   </si>
 </sst>
 </file>
@@ -524,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,23 +979,47 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
       <c r="B39">
         <v>37</v>
       </c>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
       <c r="B40">
         <v>38</v>
       </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
       <c r="B41">
         <v>39</v>
       </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
       <c r="B42">
         <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated opcodes 35/36 packet format to support the added IO pins.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -180,12 +180,6 @@
     <t>Set IO pin state</t>
   </si>
   <si>
-    <t>5-bit cmd, 17-bit reply</t>
-  </si>
-  <si>
-    <t>17-bit</t>
-  </si>
-  <si>
     <t>Get U15 output pin X</t>
   </si>
   <si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>8-bit command</t>
+  </si>
+  <si>
+    <t>6-bit cmd, 18-bit reply</t>
+  </si>
+  <si>
+    <t>8-bit</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,51 +975,51 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed U15 to U16.
</commit_message>
<xml_diff>
--- a/Documentation/XMOS-STM32-UART.xlsx
+++ b/Documentation/XMOS-STM32-UART.xlsx
@@ -180,18 +180,6 @@
     <t>Set IO pin state</t>
   </si>
   <si>
-    <t>Get U15 output pin X</t>
-  </si>
-  <si>
-    <t>Set U15 output pin X</t>
-  </si>
-  <si>
-    <t>Get U15 outputs</t>
-  </si>
-  <si>
-    <t>Set U15 outputs</t>
-  </si>
-  <si>
     <t>3-bit cmd, 1-bit reply</t>
   </si>
   <si>
@@ -208,6 +196,18 @@
   </si>
   <si>
     <t>8-bit</t>
+  </si>
+  <si>
+    <t>Set U16 outputs</t>
+  </si>
+  <si>
+    <t>Get U16 outputs</t>
+  </si>
+  <si>
+    <t>Set U16 output pin X</t>
+  </si>
+  <si>
+    <t>Get U16 output pin X</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,51 +975,51 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
         <v>55</v>
-      </c>
-      <c r="B40">
-        <v>38</v>
-      </c>
-      <c r="D40" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>